<commit_message>
Use a more lenient test for Schur decomposition
</commit_message>
<xml_diff>
--- a/jacobi/src/test/resources/jacobi/test/data/SchurDecompTest.xlsx
+++ b/jacobi/src/test/resources/jacobi/test/data/SchurDecompTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="240" windowWidth="27795" windowHeight="12555" activeTab="3"/>
+    <workbookView xWindow="630" yWindow="240" windowWidth="27795" windowHeight="12555"/>
   </bookViews>
   <sheets>
     <sheet name="4x4" sheetId="1" r:id="rId1"/>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,16 +492,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2.24073811167673</v>
+        <v>2.24073811167671</v>
       </c>
       <c r="B10">
-        <v>-4.57715763663695</v>
+        <v>-4.5771576366369304</v>
       </c>
       <c r="C10">
-        <v>-4.6785630403706602</v>
+        <v>-4.67856303151137</v>
       </c>
       <c r="D10">
-        <v>0.67665138260851498</v>
+        <v>0.67665144386405696</v>
       </c>
       <c r="G10" t="s">
         <v>10</v>
@@ -515,28 +515,28 @@
       </c>
       <c r="K10">
         <f>H10*H10-4*H11</f>
-        <v>-17.569050697776518</v>
+        <v>-17.569050697776234</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>1.8627006121276599</v>
+        <v>1.8627006121276699</v>
       </c>
       <c r="B11">
-        <v>6.30699519018237</v>
+        <v>6.3069951901823904</v>
       </c>
       <c r="C11">
-        <v>3.37264862138246</v>
+        <v>3.3726486057113001</v>
       </c>
       <c r="D11">
-        <v>-1.1969301476471399</v>
+        <v>-1.19693019180459</v>
       </c>
       <c r="G11" t="s">
         <v>9</v>
       </c>
       <c r="H11">
         <f>A10*B11-A11*B10</f>
-        <v>22.658198824371901</v>
+        <v>22.65819882437183</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -544,13 +544,13 @@
         <v>0</v>
       </c>
       <c r="B12" s="1">
-        <v>1.07550293898039E-14</v>
+        <v>1.0755029440950899E-14</v>
       </c>
       <c r="C12">
-        <v>6.3266905340232302</v>
+        <v>6.3266905275233496</v>
       </c>
       <c r="D12">
-        <v>2.10789016489188</v>
+        <v>2.1078901768269498</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -558,13 +558,13 @@
         <v>0</v>
       </c>
       <c r="B13" s="1">
-        <v>-7.8886090522101102E-31</v>
+        <v>0</v>
       </c>
       <c r="C13">
-        <v>-2.6043370750090502</v>
+        <v>-2.6043370630739799</v>
       </c>
       <c r="D13">
-        <v>7.2382648213738197</v>
+        <v>7.2382648278737101</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -585,58 +585,58 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>0.16875417142253299</v>
+        <v>-0.16875417142253701</v>
       </c>
       <c r="B17">
-        <v>0.952645031321247</v>
+        <v>-0.95264503132124601</v>
       </c>
       <c r="C17">
-        <v>-0.19258058042658699</v>
+        <v>0.192580582574055</v>
       </c>
       <c r="D17">
-        <v>-0.16401888296471401</v>
+        <v>0.16401888044329199</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>-0.82878306706916904</v>
+        <v>0.82878306706916804</v>
       </c>
       <c r="B18">
-        <v>0.260422163601429</v>
+        <v>-0.260422163601433</v>
       </c>
       <c r="C18">
-        <v>0.48748985159840003</v>
+        <v>-0.48748985274374501</v>
       </c>
       <c r="D18">
-        <v>8.7478963374865396E-2</v>
+        <v>-8.7478956992252097E-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.50681118568456596</v>
+        <v>-0.50681118568456596</v>
       </c>
       <c r="B19">
-        <v>0.135011962310535</v>
+        <v>-0.135011962310532</v>
       </c>
       <c r="C19">
-        <v>0.70342677056089098</v>
+        <v>-0.70342677684141597</v>
       </c>
       <c r="D19">
-        <v>0.47969257921750103</v>
+        <v>-0.47969257000766602</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>-0.16668257087025901</v>
+        <v>0.16668257087025901</v>
       </c>
       <c r="B20">
-        <v>8.0121851183984405E-2</v>
+        <v>-8.0121851183985293E-2</v>
       </c>
       <c r="C20">
-        <v>-0.48005952036117799</v>
+        <v>0.480059509133831</v>
       </c>
       <c r="D20">
-        <v>0.85751983443039204</v>
+        <v>-0.85751984071572096</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -652,41 +652,41 @@
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="array" ref="A24:D27">MMULT(A17:D20,TRANSPOSE(A17:D20))</f>
-        <v>0.999999999999999</v>
+        <v>0.999999999999998</v>
       </c>
       <c r="B24">
-        <v>-1.3877787807814457E-16</v>
+        <v>6.2450045135165055E-16</v>
       </c>
       <c r="C24">
-        <v>-5.5511151231257827E-17</v>
+        <v>-3.8857805861880479E-16</v>
       </c>
       <c r="D24">
-        <v>1.3877787807814457E-16</v>
+        <v>4.4408920985006262E-16</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>-1.3877787807814457E-16</v>
+        <v>6.2450045135165055E-16</v>
       </c>
       <c r="B25">
-        <v>0.99999999999999933</v>
+        <v>0.99999999999999911</v>
       </c>
       <c r="C25">
-        <v>4.0939474033052647E-16</v>
+        <v>2.3592239273284576E-16</v>
       </c>
       <c r="D25">
-        <v>-5.4123372450476381E-16</v>
+        <v>3.4694469519536142E-16</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>-5.5511151231257827E-17</v>
+        <v>-3.8857805861880479E-16</v>
       </c>
       <c r="B26">
-        <v>4.0939474033052647E-16</v>
+        <v>2.3592239273284576E-16</v>
       </c>
       <c r="C26">
-        <v>0.99999999999999978</v>
+        <v>0.99999999999999889</v>
       </c>
       <c r="D26">
         <v>1.6653345369377348E-16</v>
@@ -694,16 +694,16 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>1.3877787807814457E-16</v>
+        <v>4.4408920985006262E-16</v>
       </c>
       <c r="B27">
-        <v>-5.4123372450476381E-16</v>
+        <v>3.4694469519536142E-16</v>
       </c>
       <c r="C27">
         <v>1.6653345369377348E-16</v>
       </c>
       <c r="D27">
-        <v>0.99999999999999867</v>
+        <v>0.99999999999999789</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -717,54 +717,54 @@
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="array" ref="A30:D33">MMULT(A17:D20,MMULT(A10:D13,TRANSPOSE(A17:D20)))</f>
-        <v>5.4665069389323877</v>
+        <v>5.4665069389323886</v>
       </c>
       <c r="B30">
-        <v>0.14602913571357978</v>
+        <v>0.14602913571359283</v>
       </c>
       <c r="C30">
-        <v>1.689583112391376</v>
+        <v>1.6895831123913747</v>
       </c>
       <c r="D30">
-        <v>-2.9688610466534238</v>
+        <v>-2.9688610466534104</v>
       </c>
       <c r="F30">
         <f>A30-A3</f>
-        <v>-1.6875389974302379E-14</v>
+        <v>-1.5987211554602254E-14</v>
       </c>
       <c r="G30">
         <f t="shared" ref="G30:I30" si="0">B30-B3</f>
-        <v>-4.1078251911130792E-15</v>
+        <v>8.9372953482325102E-15</v>
       </c>
       <c r="H30">
         <f t="shared" si="0"/>
-        <v>2.6645352591003757E-15</v>
+        <v>0</v>
       </c>
       <c r="I30">
         <f t="shared" si="0"/>
-        <v>6.2172489379008766E-15</v>
+        <v>1.9539925233402755E-14</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>3.3517501610040616</v>
+        <v>3.3517501610040701</v>
       </c>
       <c r="B31">
-        <v>6.3325570231753421</v>
+        <v>6.3325570231753341</v>
       </c>
       <c r="C31">
-        <v>5.7713251950410305</v>
+        <v>5.7713251950410287</v>
       </c>
       <c r="D31">
-        <v>-2.3141277615050804</v>
+        <v>-2.3141277615050742</v>
       </c>
       <c r="F31">
         <f t="shared" ref="F31:F33" si="1">A31-A4</f>
-        <v>-7.9936057773011271E-15</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <f t="shared" ref="G31:G33" si="2">B31-B4</f>
-        <v>0</v>
+        <v>-1.1546319456101628E-14</v>
       </c>
       <c r="H31">
         <f t="shared" ref="H31:H33" si="3">C31-C4</f>
@@ -772,67 +772,67 @@
       </c>
       <c r="I31">
         <f t="shared" ref="I31:I33" si="4">D31-D4</f>
-        <v>0</v>
+        <v>5.773159728050814E-15</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>-2.2545826492028391</v>
+        <v>-2.2545826492028387</v>
       </c>
       <c r="B32">
-        <v>-0.45610736259196094</v>
+        <v>-0.45610736259195273</v>
       </c>
       <c r="C32">
-        <v>3.8726875251172688</v>
+        <v>3.8726875251172705</v>
       </c>
       <c r="D32">
-        <v>3.4385549813766225</v>
+        <v>3.4385549813766199</v>
       </c>
       <c r="F32">
         <f t="shared" si="1"/>
-        <v>3.5527136788005009E-15</v>
+        <v>3.9968028886505635E-15</v>
       </c>
       <c r="G32">
         <f t="shared" si="2"/>
-        <v>6.6613381477509392E-16</v>
+        <v>8.8817841970012523E-15</v>
       </c>
       <c r="H32">
         <f t="shared" si="3"/>
-        <v>-7.1054273576010019E-15</v>
+        <v>-5.3290705182007514E-15</v>
       </c>
       <c r="I32">
         <f t="shared" si="4"/>
-        <v>-8.8817841970012523E-15</v>
+        <v>-1.1546319456101628E-14</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>1.1652697618504186</v>
+        <v>1.1652697618504213</v>
       </c>
       <c r="B33">
-        <v>-1.105064424135471</v>
+        <v>-1.1050644241354663</v>
       </c>
       <c r="C33">
-        <v>-0.51924626934742046</v>
+        <v>-0.51924626934741891</v>
       </c>
       <c r="D33">
-        <v>6.4409371700311366</v>
+        <v>6.4409371700311358</v>
       </c>
       <c r="F33">
         <f t="shared" si="1"/>
-        <v>-4.4408920985006262E-15</v>
+        <v>-1.7763568394002505E-15</v>
       </c>
       <c r="G33">
         <f t="shared" si="2"/>
-        <v>-3.5527136788005009E-15</v>
+        <v>0</v>
       </c>
       <c r="H33">
         <f t="shared" si="3"/>
-        <v>-2.4424906541753444E-15</v>
+        <v>-8.8817841970012523E-16</v>
       </c>
       <c r="I33">
         <f t="shared" si="4"/>
-        <v>-1.3322676295501878E-14</v>
+        <v>-1.4210854715202004E-14</v>
       </c>
     </row>
   </sheetData>
@@ -1561,7 +1561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A21" sqref="A21:G26"/>
     </sheetView>
   </sheetViews>
@@ -2415,951 +2415,951 @@
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <f ca="1">RAND()*10-3</f>
-        <v>-0.6597871126734427</v>
+        <v>-0.17577599358529827</v>
       </c>
       <c r="B1">
         <f t="shared" ref="B1:I16" ca="1" si="0">RAND()*10-3</f>
-        <v>-2.2163460506341899</v>
+        <v>6.5546803484661034</v>
       </c>
       <c r="C1">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4766412438138135</v>
+        <v>-0.39431313914516108</v>
       </c>
       <c r="D1">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.6961808973160011</v>
+        <v>6.9526406394651836</v>
       </c>
       <c r="E1">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15251520122420548</v>
+        <v>-1.6683458914504774</v>
       </c>
       <c r="F1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1959156118275678</v>
+        <v>2.7287072724552921</v>
       </c>
       <c r="G1">
         <f t="shared" ca="1" si="0"/>
-        <v>-9.6996453306728903E-2</v>
+        <v>0.12366262680630591</v>
       </c>
       <c r="H1">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0013868793232596</v>
+        <v>0.79401216934366037</v>
       </c>
       <c r="I1">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2955409387978163</v>
+        <v>-1.5614771993002148</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:I25" ca="1" si="1">RAND()*10-3</f>
-        <v>0.84814488062254689</v>
+        <v>5.7136868517481503</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1152558687039189</v>
+        <v>-1.2770026297401889</v>
       </c>
       <c r="C2">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.92115531952797713</v>
+        <v>-0.41028899091951576</v>
       </c>
       <c r="D2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.461049770575475</v>
+        <v>2.2592454939272146</v>
       </c>
       <c r="E2">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1319691925019999</v>
+        <v>-1.1670140465438934</v>
       </c>
       <c r="F2">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6065535292432216</v>
+        <v>-2.3209739455470153</v>
       </c>
       <c r="G2">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2469426946986815</v>
+        <v>4.0285953857250707</v>
       </c>
       <c r="H2">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35610688178621519</v>
+        <v>0.18765862621145946</v>
       </c>
       <c r="I2">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6059400999543989</v>
+        <v>-0.3432186633436114</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2358597655791197</v>
+        <v>6.2338464834492235</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.879522848261745</v>
+        <v>4.8430702751262702</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.7308764838445807</v>
+        <v>0.84425601144564366</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11434238547646647</v>
+        <v>-1.1594094461901245</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>-5.0862454235330645E-2</v>
+        <v>1.7790748263464566</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8441351518699198</v>
+        <v>-2.1188256849717417</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1843684876062426</v>
+        <v>-0.92662045628786727</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7678584731071414</v>
+        <v>3.6738475328566151</v>
       </c>
       <c r="I3">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7826648859910506</v>
+        <v>5.3637722405242183</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0672845520223255</v>
+        <v>-2.5335698789288505</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9960264136507084</v>
+        <v>6.1803490570540482</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.7209866963375569</v>
+        <v>5.3897519862482426</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0120566226508183</v>
+        <v>6.7388531602092883</v>
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6715959377423673</v>
+        <v>-1.3666090097202339</v>
       </c>
       <c r="F4">
         <f t="shared" ca="1" si="0"/>
-        <v>0.43032983543729797</v>
+        <v>-2.1912678169977005</v>
       </c>
       <c r="G4">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3058442373125352</v>
+        <v>-0.37729892298710554</v>
       </c>
       <c r="H4">
         <f t="shared" ca="1" si="0"/>
-        <v>1.3438364064242183</v>
+        <v>-1.9172195941489441</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5916016480738504</v>
+        <v>-2.5919734397291654</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8453619465781284</v>
+        <v>4.3022505597508331</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1794815050886633</v>
+        <v>-2.8053942268417602</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.3120732067616621</v>
+        <v>-0.4920365760823171</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4667768612122263</v>
+        <v>1.6611811052866017</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>0.48787312572047981</v>
+        <v>1.7844247383258676</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2915983225771828</v>
+        <v>3.8340937049290265</v>
       </c>
       <c r="G5">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6899239076759018</v>
+        <v>-0.94527354075180714</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7147309447368801</v>
+        <v>-0.76057921240244397</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4927079996452512</v>
+        <v>5.1662992962204619</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.6539981723986914</v>
+        <v>0.84906135389886295</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6443223068122279</v>
+        <v>7.2556205238445859E-2</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62834165476476933</v>
+        <v>1.1196355158162232</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>1.1450462947428388</v>
+        <v>4.874715179578498</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0065519643738341</v>
+        <v>-0.23555149996395697</v>
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4064220904303149</v>
+        <v>3.8887724788725535</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45842397432580917</v>
+        <v>-0.73128773733584662</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1054096126583257</v>
+        <v>5.3967507884122519</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="0"/>
-        <v>2.6281333836012255</v>
+        <v>3.3913226236995611</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.508101727118107</v>
+        <v>1.5385747455343921</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9031005505652183</v>
+        <v>0.46794154430762003</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.9987557911145792</v>
+        <v>-2.5920983358691672</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3009068817212928</v>
+        <v>-0.41059195644026447</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3829658722695743</v>
+        <v>6.1835348827942926</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1443965555850433</v>
+        <v>1.900641353591098</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.56251847345585926</v>
+        <v>5.8865557670471738</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1665931944161407</v>
+        <v>2.8827061576746438</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="0"/>
-        <v>4.125339106768771</v>
+        <v>-1.601964926308665</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4074395489473543</v>
+        <v>5.1350931983709334</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8978665538879724</v>
+        <v>1.8488034317500812</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0610555833501278</v>
+        <v>4.9476652373718935</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8041914076711265</v>
+        <v>1.120651529043017</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.37187030276384325</v>
+        <v>-0.76424715407176969</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2796079749631701</v>
+        <v>6.808403869488977</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2004914558830002</v>
+        <v>2.8264105852846253</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.52550219148182631</v>
+        <v>3.9110107129014287</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8162468148351447</v>
+        <v>0.655492310821149</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.1315275970668499</v>
+        <v>4.4138983217868262</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.27833291083149181</v>
+        <v>0.62582057356783949</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5812303941582435</v>
+        <v>-2.2542879548091661</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1922490078874866</v>
+        <v>6.4205369177987599</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2134725791072674</v>
+        <v>0.83498747688974095</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8474305685748451</v>
+        <v>-2.1113338827508947</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.74538835328043707</v>
+        <v>0.33522064376931748</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3172320861601605</v>
+        <v>3.4212904027464388</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6027115974152046</v>
+        <v>-1.245285661809838</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90792966098446026</v>
+        <v>2.8976752279449718</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4163570628018181</v>
+        <v>4.3356940609547951</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0960030040238502</v>
+        <v>5.0186277953620628</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.5268215466928488</v>
+        <v>-1.342213412019559</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1075594423214681</v>
+        <v>0.13878034370499215</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.5972022749101331</v>
+        <v>6.9006852180386744</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.1337223133815462</v>
+        <v>5.0710405865340178</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.9328087328698222</v>
+        <v>9.2881980348892945E-2</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0063974736423411</v>
+        <v>-1.4747555616612225</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" ca="1" si="1"/>
-        <v>4.097863793374759</v>
+        <v>6.5998718635971052</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8914248570013648</v>
+        <v>3.2544706427872541</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.8436159243323587</v>
+        <v>-0.67111418991571892</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.24921223733135145</v>
+        <v>2.5729547776483921</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6146479324908363</v>
+        <v>-2.4481681140817964</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4309009652180649</v>
+        <v>6.7778907410575542</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>5.5582258373606894</v>
+        <v>1.9471027160905301</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.33925783197408954</v>
+        <v>3.491222371300732</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7129519438966083</v>
+        <v>3.0333098234666762</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0392218584297321</v>
+        <v>3.1759121372679573</v>
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70653395067661062</v>
+        <v>-1.73172244668458</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3530090609085379</v>
+        <v>-1.0118852842510024</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7071927039531474E-3</v>
+        <v>4.6382415847484069</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3721191298514555</v>
+        <v>-1.946817545664949</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7645148334672713</v>
+        <v>6.922754907154939</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9848530992336011</v>
+        <v>1.8690888711187874</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="0"/>
-        <v>1.817746552205965</v>
+        <v>-2.0831117711885643</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.82689336113334244</v>
+        <v>-2.6573390625408617</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.25147917842740775</v>
+        <v>0.87179533269813714</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.9342749987199988</v>
+        <v>3.6413731155787801</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.725230831063433</v>
+        <v>0.81265884055476434</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0878211426408804</v>
+        <v>4.8404285639120355</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.8570506229134631</v>
+        <v>4.2869128238452223</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.4873151464731018</v>
+        <v>5.8728405617451074</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>4.6698347089592218</v>
+        <v>-0.21614885943896445</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7837313774022707</v>
+        <v>-0.74712978017759957</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="0"/>
-        <v>4.4930103815677098</v>
+        <v>5.2122515810881236</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.2676254117342673</v>
+        <v>-0.2325136744312335</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.2417153885031169</v>
+        <v>-5.7375363530532297E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.3808609825475475</v>
+        <v>2.3295018423166383</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0308551861101325</v>
+        <v>-2.7028946326781931</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.3037261220937495</v>
+        <v>3.716336306141212</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.2066816278458998</v>
+        <v>3.0558960544744442</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4255912768886276</v>
+        <v>5.5801413203118617</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1716874776054951</v>
+        <v>-2.2298683498753107</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.16436268158598732</v>
+        <v>6.0027335988088133</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.8355484401578619</v>
+        <v>3.0329148076723467</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.1496996988129544</v>
+        <v>3.4579703500357972</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.55467894177175747</v>
+        <v>-1.5949830450906517</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0882267120950129</v>
+        <v>5.3979971504169431</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.8390797040611204E-2</v>
+        <v>4.4221081951722727</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8241503672914412</v>
+        <v>-2.5223359659625162</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2625768494998448</v>
+        <v>-1.3921739194716971</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5402869084590582</v>
+        <v>-2.5775356148630522</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.7363083694167076</v>
+        <v>0.20672514790102836</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" ca="1" si="1"/>
-        <v>6.5260731495007871</v>
+        <v>6.7044060024661185</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5871012758586422</v>
+        <v>2.1078886094004812</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0978276720794629</v>
+        <v>-1.2840696709203232</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.49682662960309054</v>
+        <v>-1.2014729006161646</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.5170167079829926</v>
+        <v>5.8878176113503073</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9110823517396005</v>
+        <v>-2.5085859970477262</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>5.8411053734767133</v>
+        <v>-1.3769746543880186</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1325394743287163</v>
+        <v>4.146701255949699</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.5568339858854321</v>
+        <v>2.2649878175316687</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5684670857561267</v>
+        <v>5.367426203343129</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6081146612293908</v>
+        <v>-1.5589113833962394</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>3.3462645011750656</v>
+        <v>2.2723143157601022</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.0124369981794494</v>
+        <v>-2.9203997173225842</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9406474527266617</v>
+        <v>6.7184307276663304</v>
       </c>
       <c r="F17">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4164340667023048</v>
+        <v>1.3592476155873472</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8894992896365501</v>
+        <v>3.861823321121074</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0488996114823355</v>
+        <v>3.240960626058448</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="1"/>
-        <v>5.2022592436977355</v>
+        <v>3.0993729865666264</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.3386983449285235</v>
+        <v>5.0157359927608454</v>
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.6336451385451047</v>
+        <v>-2.7924386730811506</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90131759335736517</v>
+        <v>2.8600033651370254</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.2618047928828062</v>
+        <v>-3.7708539154766463E-2</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1756706641023342</v>
+        <v>-2.7357825247452636</v>
       </c>
       <c r="F18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.7628566484160464</v>
+        <v>-0.88528222376959853</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5672031397493846</v>
+        <v>0.42401050228585113</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="1"/>
-        <v>6.639149212737447</v>
+        <v>3.8339293907431635</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1388519890765227</v>
+        <v>1.4738160734946897</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0407063233419489</v>
+        <v>-0.23320381027406167</v>
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4765372176217877</v>
+        <v>-2.1326386612109731</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.6985870659464184</v>
+        <v>4.9151585919568603</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5041863161272131</v>
+        <v>-2.69745209628325</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2911721230912772</v>
+        <v>-2.3000769938174157</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.8753936834549085</v>
+        <v>-1.2683524330762947</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="1"/>
-        <v>5.538562888256525</v>
+        <v>5.3345815464299235</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="1"/>
-        <v>2.784307547045727</v>
+        <v>-1.6021868910122068</v>
       </c>
       <c r="I19">
         <f t="shared" ca="1" si="1"/>
-        <v>0.47054693275056358</v>
+        <v>3.9207218758709912</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.9038162382829489</v>
+        <v>-0.56124689105340053</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.1945979383321186</v>
+        <v>-1.7419791193497787</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.36881157293563938</v>
+        <v>4.6063373775385932</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>6.1034117267723609</v>
+        <v>5.2585810007536278</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>0.40066515893703158</v>
+        <v>0.25635214129918715</v>
       </c>
       <c r="F20">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7351975788411647</v>
+        <v>6.4371168092886517</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4177610753870828</v>
+        <v>5.7852291090118833</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>4.611982722484556</v>
+        <v>-1.0513437631520512</v>
       </c>
       <c r="I20">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1316486500484277</v>
+        <v>2.9132258045655819</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" ca="1" si="1"/>
-        <v>3.2835933497594922</v>
+        <v>3.9100390021251732</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.75500464580168503</v>
+        <v>0.12040038452202939</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>0.17315634979840411</v>
+        <v>5.922465267415765</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>2.255692202510474</v>
+        <v>-1.5176623037797028</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>5.4173874513977758</v>
+        <v>5.5773910714873409</v>
       </c>
       <c r="F21">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8926115238052912</v>
+        <v>-1.6288501587901467</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9011754647132113</v>
+        <v>-2.0356095986426901</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>3.5095688192842962</v>
+        <v>1.7418304542040044</v>
       </c>
       <c r="I21">
         <f t="shared" ca="1" si="1"/>
-        <v>6.7558327597697243</v>
+        <v>3.5171717945582035</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" ca="1" si="1"/>
-        <v>2.2901587257003708</v>
+        <v>5.2125047195434497</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>6.6366974554553959</v>
+        <v>3.45590805811604</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8983824003472485</v>
+        <v>-1.4720414565359459</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4547135016121562</v>
+        <v>-2.4504372784081605</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5195849290631092</v>
+        <v>0.11431557034209217</v>
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.81824567703997753</v>
+        <v>-2.3934232794385455</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>4.2808625954929784</v>
+        <v>-2.7786830329622756</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.67938861681859075</v>
+        <v>5.5159646558710573</v>
       </c>
       <c r="I22">
         <f t="shared" ca="1" si="1"/>
-        <v>0.90457338436169721</v>
+        <v>3.1503203997398881</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" ca="1" si="1"/>
-        <v>3.4698955911575586</v>
+        <v>1.1084626502019441</v>
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="1"/>
-        <v>2.0363563546802839</v>
+        <v>-0.5109838896420289</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4217686623054124</v>
+        <v>-2.3065974552569202E-2</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6302626458543745</v>
+        <v>1.562785116472865</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.5085744086834403</v>
+        <v>-1.4739348040933049</v>
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6803315190971704</v>
+        <v>3.5305654740888377</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.690902357164624</v>
+        <v>2.6432548354606205</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>4.6987249527639232</v>
+        <v>4.2074325816823706</v>
       </c>
       <c r="I23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8887567338400011</v>
+        <v>2.4501098427228589</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" ca="1" si="1"/>
-        <v>0.20270737670373284</v>
+        <v>3.6183203273445361</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.4857580661011132</v>
+        <v>1.3565366940673353</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.8753899939658498</v>
+        <v>0.86368481963126564</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1893459660048977</v>
+        <v>6.1339580167190899</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.6644893963989222E-2</v>
+        <v>0.68376513952094786</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
-        <v>5.1056599323392735</v>
+        <v>2.9153002528139655</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.2208234629133381</v>
+        <v>-2.0711716828007849</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="1"/>
-        <v>4.9108946962638305</v>
+        <v>4.0949113937573669</v>
       </c>
       <c r="I24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.7270125428480112</v>
+        <v>5.0197498648844654</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.1842709040500567</v>
+        <v>6.686219687574452</v>
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0956985995483404</v>
+        <v>5.9370464774408021</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.89558605744343023</v>
+        <v>3.7925981605191783E-2</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.7386086995218282</v>
+        <v>-0.92592035405684481</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0154277985378108</v>
+        <v>3.3814642918611231</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.2537023013183064</v>
+        <v>3.9500398234611609</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.737412542515739</v>
+        <v>0.27943607123166636</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.9376899323230123</v>
+        <v>1.3970196249635105</v>
       </c>
       <c r="I25">
         <f t="shared" ca="1" si="1"/>
-        <v>0.54114961491845204</v>
+        <v>0.36743574086951014</v>
       </c>
     </row>
   </sheetData>

</xml_diff>